<commit_message>
Adelanto del CU- consultar información de maestro
Se hizo un adelanto en el caso de uso consultar información de maestro, así como también se hizo el registro de los tiempos que se llevaron hasta ahora en las plantillas de tareas y de casos de uso
</commit_message>
<xml_diff>
--- a/Plantillas/Entrega 3/Plantilla Lista de Tareas de la Entrega 3.xlsx
+++ b/Plantillas/Entrega 3/Plantilla Lista de Tareas de la Entrega 3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iro19\Documents\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irdev\OneDrive\Documentos\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12F65CC-2636-436B-9835-45BE84AED431}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535311BD-2E96-4E4F-B0D4-95FCC1CD1324}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="69">
   <si>
     <t>Columna</t>
   </si>
@@ -235,6 +235,12 @@
   </si>
   <si>
     <t>Prueba unitaria</t>
+  </si>
+  <si>
+    <t>Hecho</t>
+  </si>
+  <si>
+    <t>En proceso</t>
   </si>
 </sst>
 </file>
@@ -531,15 +537,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -551,6 +548,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -899,10 +905,10 @@
   <dimension ref="B1:BJ28"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="AW21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="AX26" sqref="AX26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,100 +990,100 @@
       <c r="BI3" s="2"/>
     </row>
     <row r="4" spans="2:62" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H4" s="46" t="s">
+      <c r="H4" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="47"/>
+      <c r="I4" s="53"/>
       <c r="J4" s="8"/>
-      <c r="K4" s="46" t="s">
+      <c r="K4" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="47"/>
+      <c r="L4" s="53"/>
       <c r="M4" s="8"/>
-      <c r="N4" s="46" t="s">
+      <c r="N4" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="47"/>
+      <c r="O4" s="53"/>
       <c r="P4" s="8"/>
-      <c r="Q4" s="46" t="s">
+      <c r="Q4" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="47"/>
+      <c r="R4" s="53"/>
       <c r="S4" s="8"/>
-      <c r="T4" s="46" t="s">
+      <c r="T4" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="U4" s="47"/>
+      <c r="U4" s="53"/>
       <c r="V4" s="8"/>
-      <c r="W4" s="46" t="s">
+      <c r="W4" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="X4" s="47"/>
+      <c r="X4" s="53"/>
       <c r="Y4" s="8"/>
-      <c r="Z4" s="46" t="s">
+      <c r="Z4" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="AA4" s="47"/>
+      <c r="AA4" s="53"/>
       <c r="AB4" s="8"/>
-      <c r="AC4" s="46" t="s">
+      <c r="AC4" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="AD4" s="47"/>
+      <c r="AD4" s="53"/>
       <c r="AE4" s="8"/>
-      <c r="AF4" s="46" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG4" s="47"/>
+      <c r="AF4" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG4" s="53"/>
       <c r="AH4" s="8"/>
-      <c r="AI4" s="46" t="s">
+      <c r="AI4" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="AJ4" s="47"/>
+      <c r="AJ4" s="53"/>
       <c r="AK4" s="8"/>
-      <c r="AL4" s="46" t="s">
+      <c r="AL4" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="AM4" s="47"/>
+      <c r="AM4" s="53"/>
       <c r="AN4" s="8"/>
-      <c r="AO4" s="46" t="s">
+      <c r="AO4" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="AP4" s="47"/>
+      <c r="AP4" s="53"/>
       <c r="AQ4" s="8"/>
-      <c r="AR4" s="46" t="s">
+      <c r="AR4" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="AS4" s="47"/>
+      <c r="AS4" s="53"/>
       <c r="AT4" s="8"/>
-      <c r="AU4" s="46" t="s">
+      <c r="AU4" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="AV4" s="47"/>
+      <c r="AV4" s="53"/>
       <c r="AW4" s="8"/>
-      <c r="AX4" s="46" t="s">
+      <c r="AX4" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="AY4" s="47"/>
-      <c r="AZ4" s="46" t="s">
+      <c r="AY4" s="53"/>
+      <c r="AZ4" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="BA4" s="48"/>
-      <c r="BB4" s="48" t="s">
+      <c r="BA4" s="54"/>
+      <c r="BB4" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="BC4" s="48"/>
-      <c r="BD4" s="48" t="s">
+      <c r="BC4" s="54"/>
+      <c r="BD4" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="BE4" s="48"/>
-      <c r="BF4" s="48" t="s">
+      <c r="BE4" s="54"/>
+      <c r="BF4" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="BG4" s="47"/>
-      <c r="BH4" s="46" t="s">
+      <c r="BG4" s="53"/>
+      <c r="BH4" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="BI4" s="47"/>
+      <c r="BI4" s="53"/>
     </row>
     <row r="5" spans="2:62" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
@@ -1435,7 +1441,7 @@
       <c r="C8" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D8" s="49"/>
+      <c r="D8" s="46"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
       <c r="G8" s="19"/>
@@ -1700,7 +1706,7 @@
       <c r="D11" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="50" t="s">
+      <c r="E11" s="47" t="s">
         <v>43</v>
       </c>
       <c r="F11" s="20" t="s">
@@ -1834,7 +1840,7 @@
       <c r="D12" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="E12" s="50" t="s">
+      <c r="E12" s="47" t="s">
         <v>43</v>
       </c>
       <c r="F12" s="20" t="s">
@@ -2038,7 +2044,7 @@
       <c r="D14" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="E14" s="50" t="s">
+      <c r="E14" s="47" t="s">
         <v>43</v>
       </c>
       <c r="F14" s="20" t="s">
@@ -2172,7 +2178,7 @@
       <c r="D15" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="50" t="s">
+      <c r="E15" s="47" t="s">
         <v>43</v>
       </c>
       <c r="F15" s="20" t="s">
@@ -3046,8 +3052,8 @@
       <c r="E23" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="F23" s="51" t="s">
-        <v>47</v>
+      <c r="F23" s="48" t="s">
+        <v>67</v>
       </c>
       <c r="G23" s="44">
         <v>15</v>
@@ -3088,86 +3094,96 @@
         <v>15</v>
       </c>
       <c r="Y23" s="40"/>
-      <c r="Z23" s="40"/>
+      <c r="Z23" s="40">
+        <v>2.5</v>
+      </c>
       <c r="AA23" s="40">
         <f t="shared" si="6"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="AB23" s="40"/>
       <c r="AC23" s="40"/>
       <c r="AD23" s="40">
         <f t="shared" si="7"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="AE23" s="40"/>
       <c r="AF23" s="40"/>
       <c r="AG23" s="40">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="AH23" s="40"/>
-      <c r="AI23" s="40"/>
+      <c r="AI23" s="40">
+        <v>1</v>
+      </c>
       <c r="AJ23" s="40">
         <f t="shared" si="9"/>
-        <v>15</v>
+        <v>11.5</v>
       </c>
       <c r="AK23" s="40"/>
-      <c r="AL23" s="40"/>
+      <c r="AL23" s="40">
+        <v>1</v>
+      </c>
       <c r="AM23" s="40">
         <f t="shared" si="10"/>
-        <v>15</v>
+        <v>10.5</v>
       </c>
       <c r="AN23" s="40"/>
-      <c r="AO23" s="40"/>
+      <c r="AO23" s="40">
+        <v>4</v>
+      </c>
       <c r="AP23" s="40">
         <f t="shared" si="11"/>
-        <v>15</v>
+        <v>6.5</v>
       </c>
       <c r="AQ23" s="40"/>
-      <c r="AR23" s="40"/>
+      <c r="AR23" s="40">
+        <v>2.5</v>
+      </c>
       <c r="AS23" s="40">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="AT23" s="40"/>
       <c r="AU23" s="40"/>
       <c r="AV23" s="40">
         <f t="shared" si="13"/>
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="AW23" s="40"/>
       <c r="AX23" s="40"/>
       <c r="AY23" s="40">
         <f t="shared" si="19"/>
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="AZ23" s="40"/>
       <c r="BA23" s="40">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="BB23" s="40"/>
       <c r="BC23" s="40">
         <f t="shared" si="15"/>
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="BD23" s="40"/>
       <c r="BE23" s="40">
         <f t="shared" si="16"/>
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="BF23" s="40"/>
       <c r="BG23" s="40">
         <f t="shared" si="17"/>
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="BH23" s="36">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="BI23" s="36">
         <f>G23-BH23</f>
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="BJ23" s="2"/>
     </row>
@@ -3180,7 +3196,7 @@
       <c r="E24" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="F24" s="51" t="s">
+      <c r="F24" s="48" t="s">
         <v>47</v>
       </c>
       <c r="G24" s="44">
@@ -3382,7 +3398,7 @@
         <v>46</v>
       </c>
       <c r="F26" s="40" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="G26" s="44">
         <v>15</v>
@@ -3471,38 +3487,40 @@
         <v>15</v>
       </c>
       <c r="AW26" s="40"/>
-      <c r="AX26" s="40"/>
+      <c r="AX26" s="40">
+        <v>2</v>
+      </c>
       <c r="AY26" s="40">
         <f t="shared" si="19"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AZ26" s="40"/>
       <c r="BA26" s="40">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="BB26" s="40"/>
       <c r="BC26" s="40">
         <f t="shared" si="15"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="BD26" s="40"/>
       <c r="BE26" s="40">
         <f t="shared" si="16"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="BF26" s="40"/>
       <c r="BG26" s="40">
         <f t="shared" si="17"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="BH26" s="36">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BI26" s="36">
         <f>G26-BH26</f>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="BJ26" s="2"/>
     </row>
@@ -3641,12 +3659,12 @@
       <c r="BJ27" s="2"/>
     </row>
     <row r="28" spans="2:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="52"/>
+      <c r="B28" s="49"/>
       <c r="C28" s="12"/>
-      <c r="D28" s="53"/>
+      <c r="D28" s="50"/>
       <c r="E28" s="5"/>
       <c r="F28" s="14"/>
-      <c r="G28" s="54"/>
+      <c r="G28" s="51"/>
       <c r="H28" s="14"/>
       <c r="I28" s="14"/>
       <c r="J28" s="15"/>
@@ -3704,6 +3722,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="BH4:BI4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="BB4:BC4"/>
+    <mergeCell ref="BD4:BE4"/>
+    <mergeCell ref="BF4:BG4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -3715,15 +3742,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="BH4:BI4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="BB4:BC4"/>
-    <mergeCell ref="BD4:BE4"/>
-    <mergeCell ref="BF4:BG4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="50" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Termino del CU Consultar informacion maestro
Se termino el CU consultar informaición del maestro, se añadi+o el plan de pruebas sobre los métodos que se conectan con la BD y se crearon las pruebas unitarias
</commit_message>
<xml_diff>
--- a/Plantillas/Entrega 3/Plantilla Lista de Tareas de la Entrega 3.xlsx
+++ b/Plantillas/Entrega 3/Plantilla Lista de Tareas de la Entrega 3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irdev\OneDrive\Documentos\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535311BD-2E96-4E4F-B0D4-95FCC1CD1324}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF2CEB2-0755-4B54-AA6B-5E2D9F1D869D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="2">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="68">
   <si>
     <t>Columna</t>
   </si>
@@ -238,9 +238,6 @@
   </si>
   <si>
     <t>Hecho</t>
-  </si>
-  <si>
-    <t>En proceso</t>
   </si>
 </sst>
 </file>
@@ -420,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -541,7 +538,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -905,10 +901,10 @@
   <dimension ref="B1:BJ28"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="AW21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="BD18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AX26" sqref="AX26"/>
+      <selection pane="bottomRight" activeCell="BH24" sqref="BH24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -990,100 +986,100 @@
       <c r="BI3" s="2"/>
     </row>
     <row r="4" spans="2:62" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H4" s="52" t="s">
+      <c r="H4" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="53"/>
+      <c r="I4" s="52"/>
       <c r="J4" s="8"/>
-      <c r="K4" s="52" t="s">
+      <c r="K4" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="53"/>
+      <c r="L4" s="52"/>
       <c r="M4" s="8"/>
-      <c r="N4" s="52" t="s">
+      <c r="N4" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="53"/>
+      <c r="O4" s="52"/>
       <c r="P4" s="8"/>
-      <c r="Q4" s="52" t="s">
+      <c r="Q4" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="53"/>
+      <c r="R4" s="52"/>
       <c r="S4" s="8"/>
-      <c r="T4" s="52" t="s">
+      <c r="T4" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="U4" s="53"/>
+      <c r="U4" s="52"/>
       <c r="V4" s="8"/>
-      <c r="W4" s="52" t="s">
+      <c r="W4" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="X4" s="53"/>
+      <c r="X4" s="52"/>
       <c r="Y4" s="8"/>
-      <c r="Z4" s="52" t="s">
+      <c r="Z4" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="AA4" s="53"/>
+      <c r="AA4" s="52"/>
       <c r="AB4" s="8"/>
-      <c r="AC4" s="52" t="s">
+      <c r="AC4" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="AD4" s="53"/>
+      <c r="AD4" s="52"/>
       <c r="AE4" s="8"/>
-      <c r="AF4" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG4" s="53"/>
+      <c r="AF4" s="51" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG4" s="52"/>
       <c r="AH4" s="8"/>
-      <c r="AI4" s="52" t="s">
+      <c r="AI4" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="AJ4" s="53"/>
+      <c r="AJ4" s="52"/>
       <c r="AK4" s="8"/>
-      <c r="AL4" s="52" t="s">
+      <c r="AL4" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="AM4" s="53"/>
+      <c r="AM4" s="52"/>
       <c r="AN4" s="8"/>
-      <c r="AO4" s="52" t="s">
+      <c r="AO4" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="AP4" s="53"/>
+      <c r="AP4" s="52"/>
       <c r="AQ4" s="8"/>
-      <c r="AR4" s="52" t="s">
+      <c r="AR4" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="AS4" s="53"/>
+      <c r="AS4" s="52"/>
       <c r="AT4" s="8"/>
-      <c r="AU4" s="52" t="s">
+      <c r="AU4" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="AV4" s="53"/>
+      <c r="AV4" s="52"/>
       <c r="AW4" s="8"/>
-      <c r="AX4" s="52" t="s">
+      <c r="AX4" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="AY4" s="53"/>
-      <c r="AZ4" s="52" t="s">
+      <c r="AY4" s="52"/>
+      <c r="AZ4" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="BA4" s="54"/>
-      <c r="BB4" s="54" t="s">
+      <c r="BA4" s="53"/>
+      <c r="BB4" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="BC4" s="54"/>
-      <c r="BD4" s="54" t="s">
+      <c r="BC4" s="53"/>
+      <c r="BD4" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="BE4" s="54"/>
-      <c r="BF4" s="54" t="s">
+      <c r="BE4" s="53"/>
+      <c r="BF4" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="BG4" s="53"/>
-      <c r="BH4" s="52" t="s">
+      <c r="BG4" s="52"/>
+      <c r="BH4" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="BI4" s="53"/>
+      <c r="BI4" s="52"/>
     </row>
     <row r="5" spans="2:62" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
@@ -3052,7 +3048,7 @@
       <c r="E23" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="F23" s="48" t="s">
+      <c r="F23" s="43" t="s">
         <v>67</v>
       </c>
       <c r="G23" s="44">
@@ -3196,8 +3192,8 @@
       <c r="E24" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="F24" s="48" t="s">
-        <v>47</v>
+      <c r="F24" s="43" t="s">
+        <v>67</v>
       </c>
       <c r="G24" s="44">
         <v>3</v>
@@ -3291,33 +3287,37 @@
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
-      <c r="AZ24" s="40"/>
+      <c r="AZ24" s="40">
+        <v>0.5</v>
+      </c>
       <c r="BA24" s="40">
         <f t="shared" si="14"/>
-        <v>3</v>
-      </c>
-      <c r="BB24" s="40"/>
+        <v>2.5</v>
+      </c>
+      <c r="BB24" s="40">
+        <v>1</v>
+      </c>
       <c r="BC24" s="40">
         <f t="shared" si="15"/>
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="BD24" s="40"/>
       <c r="BE24" s="40">
         <f t="shared" si="16"/>
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="BF24" s="40"/>
       <c r="BG24" s="40">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="BH24" s="36">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="BI24" s="36">
         <f>G24-BH24</f>
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="BJ24" s="2"/>
     </row>
@@ -3398,7 +3398,7 @@
         <v>46</v>
       </c>
       <c r="F26" s="40" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G26" s="44">
         <v>15</v>
@@ -3494,33 +3494,35 @@
         <f t="shared" si="19"/>
         <v>13</v>
       </c>
-      <c r="AZ26" s="40"/>
+      <c r="AZ26" s="40">
+        <v>6</v>
+      </c>
       <c r="BA26" s="40">
         <f t="shared" si="14"/>
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="BB26" s="40"/>
       <c r="BC26" s="40">
         <f t="shared" si="15"/>
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="BD26" s="40"/>
       <c r="BE26" s="40">
         <f t="shared" si="16"/>
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="BF26" s="40"/>
       <c r="BG26" s="40">
         <f t="shared" si="17"/>
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="BH26" s="36">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="BI26" s="36">
         <f>G26-BH26</f>
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="BJ26" s="2"/>
     </row>
@@ -3534,7 +3536,7 @@
         <v>46</v>
       </c>
       <c r="F27" s="40" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="G27" s="44">
         <v>3</v>
@@ -3628,43 +3630,47 @@
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
-      <c r="AZ27" s="40"/>
+      <c r="AZ27" s="40">
+        <v>0.5</v>
+      </c>
       <c r="BA27" s="40">
         <f t="shared" si="14"/>
-        <v>3</v>
-      </c>
-      <c r="BB27" s="40"/>
+        <v>2.5</v>
+      </c>
+      <c r="BB27" s="40">
+        <v>1</v>
+      </c>
       <c r="BC27" s="40">
         <f t="shared" si="15"/>
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="BD27" s="40"/>
       <c r="BE27" s="40">
         <f t="shared" si="16"/>
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="BF27" s="40"/>
       <c r="BG27" s="40">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="BH27" s="36">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="BI27" s="36">
         <f>G27-BH27</f>
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="BJ27" s="2"/>
     </row>
     <row r="28" spans="2:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="49"/>
+      <c r="B28" s="48"/>
       <c r="C28" s="12"/>
-      <c r="D28" s="50"/>
+      <c r="D28" s="49"/>
       <c r="E28" s="5"/>
       <c r="F28" s="14"/>
-      <c r="G28" s="51"/>
+      <c r="G28" s="50"/>
       <c r="H28" s="14"/>
       <c r="I28" s="14"/>
       <c r="J28" s="15"/>
@@ -3722,15 +3728,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="BH4:BI4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="BB4:BC4"/>
-    <mergeCell ref="BD4:BE4"/>
-    <mergeCell ref="BF4:BG4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -3742,6 +3739,15 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="BH4:BI4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="BB4:BC4"/>
+    <mergeCell ref="BD4:BE4"/>
+    <mergeCell ref="BF4:BG4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="50" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Detalles de CU 6 y 8
Se afinaron algunos detalles de ambos casos de uso, además de que se corrigió un bug que evitaba poner las fotos de los alumnos y maestros registrados
</commit_message>
<xml_diff>
--- a/Plantillas/Entrega 3/Plantilla Lista de Tareas de la Entrega 3.xlsx
+++ b/Plantillas/Entrega 3/Plantilla Lista de Tareas de la Entrega 3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Equipo\Documents\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iro19\Documents\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250FB019-A504-4A0A-BD3A-0793BDAE388E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD997F91-129D-42FA-95B2-3DBDFF4F891E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="67">
   <si>
     <t>Columna</t>
   </si>
@@ -173,9 +173,6 @@
   </si>
   <si>
     <t>IRVIN VERA</t>
-  </si>
-  <si>
-    <t>Por iniciar</t>
   </si>
   <si>
     <t>CU-06</t>
@@ -890,7 +887,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -901,13 +898,13 @@
   <dimension ref="B1:BJ28"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="BB12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="BA10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomRight" activeCell="BH14" sqref="BH14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" style="2" customWidth="1"/>
@@ -1061,19 +1058,19 @@
       </c>
       <c r="AY4" s="52"/>
       <c r="AZ4" s="51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="BA4" s="53"/>
       <c r="BB4" s="53" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BC4" s="53"/>
       <c r="BD4" s="53" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BE4" s="53"/>
       <c r="BF4" s="53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="BG4" s="52"/>
       <c r="BH4" s="51" t="s">
@@ -1238,7 +1235,7 @@
     <row r="6" spans="2:62" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="18"/>
       <c r="C6" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
@@ -1303,139 +1300,143 @@
       <c r="B7" s="18"/>
       <c r="C7" s="12"/>
       <c r="D7" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="G7" s="18">
         <v>2</v>
       </c>
-      <c r="H7" s="14"/>
+      <c r="H7" s="14">
+        <v>2</v>
+      </c>
       <c r="I7" s="14">
         <f t="shared" ref="I7:I27" si="0">G7-H7</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J7" s="15"/>
-      <c r="K7" s="14"/>
+      <c r="K7" s="14">
+        <v>1</v>
+      </c>
       <c r="L7" s="14">
         <f t="shared" ref="L7:L27" si="1">I7-K7</f>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="M7" s="15"/>
       <c r="N7" s="14"/>
       <c r="O7" s="14">
         <f t="shared" ref="O7:O27" si="2">L7-N7</f>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="P7" s="15"/>
       <c r="Q7" s="14"/>
       <c r="R7" s="14">
         <f t="shared" ref="R7:R27" si="3">O7-Q7</f>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="S7" s="15"/>
       <c r="T7" s="14"/>
       <c r="U7" s="14">
         <f t="shared" ref="U7:U27" si="4">R7-T7</f>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="V7" s="14"/>
       <c r="W7" s="14"/>
       <c r="X7" s="14">
         <f t="shared" ref="X7:X27" si="5">U7-W7</f>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="Y7" s="14"/>
       <c r="Z7" s="14"/>
       <c r="AA7" s="14">
         <f t="shared" ref="AA7:AA27" si="6">X7-Z7</f>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="AB7" s="14"/>
       <c r="AC7" s="14"/>
       <c r="AD7" s="14">
         <f t="shared" ref="AD7:AD27" si="7">AA7-AC7</f>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="AE7" s="14"/>
       <c r="AF7" s="14"/>
       <c r="AG7" s="14">
         <f t="shared" ref="AG7:AG27" si="8">AD7-AF7</f>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="AH7" s="14"/>
       <c r="AI7" s="14"/>
       <c r="AJ7" s="14">
         <f t="shared" ref="AJ7:AJ27" si="9">AG7-AI7</f>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="AK7" s="14"/>
       <c r="AL7" s="14"/>
       <c r="AM7" s="14">
         <f t="shared" ref="AM7:AM27" si="10">AJ7-AL7</f>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="AN7" s="14"/>
       <c r="AO7" s="14"/>
       <c r="AP7" s="14">
         <f t="shared" ref="AP7:AP27" si="11">AM7-AO7</f>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="AQ7" s="14"/>
       <c r="AR7" s="14"/>
       <c r="AS7" s="14">
         <f t="shared" ref="AS7:AS27" si="12">AP7-AR7</f>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="AT7" s="14"/>
       <c r="AU7" s="14"/>
       <c r="AV7" s="14">
         <f t="shared" ref="AV7:AV27" si="13">AS7-AU7</f>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="AW7" s="14"/>
       <c r="AX7" s="14"/>
       <c r="AY7" s="14">
         <f>AV7-AX7</f>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="AZ7" s="14"/>
       <c r="BA7" s="14">
         <f>AY7-AZ7</f>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="BB7" s="14"/>
       <c r="BC7" s="14">
         <f>BA7-BB7</f>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="BD7" s="14"/>
       <c r="BE7" s="14">
         <f>BC7-BD7</f>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="BF7" s="14"/>
       <c r="BG7" s="14">
         <f>BE7-BF7</f>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="BH7" s="36">
         <f>H7+K7+N7+Q7+T7+W7+Z7+AC7+AF7+AI7+AL7+AO7+AR7+AU7+AX7+AZ7+BB7+BD7+BF7</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BI7" s="36">
         <f>G7-BH7</f>
-        <v>2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="8" spans="2:62" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="18"/>
       <c r="C8" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" s="46"/>
       <c r="E8" s="14"/>
@@ -1500,13 +1501,13 @@
       <c r="B9" s="18"/>
       <c r="C9" s="12"/>
       <c r="D9" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="G9" s="18">
         <v>2.5</v>
@@ -1523,118 +1524,120 @@
         <v>2.5</v>
       </c>
       <c r="M9" s="15"/>
-      <c r="N9" s="14"/>
+      <c r="N9" s="14">
+        <v>2</v>
+      </c>
       <c r="O9" s="14">
         <f t="shared" si="2"/>
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="P9" s="15"/>
       <c r="Q9" s="14"/>
       <c r="R9" s="14">
         <f t="shared" si="3"/>
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="S9" s="15"/>
       <c r="T9" s="14"/>
       <c r="U9" s="14">
         <f t="shared" si="4"/>
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="V9" s="15"/>
       <c r="W9" s="14"/>
       <c r="X9" s="14">
         <f t="shared" si="5"/>
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="Y9" s="15"/>
       <c r="Z9" s="14"/>
       <c r="AA9" s="14">
         <f t="shared" si="6"/>
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="AB9" s="15"/>
       <c r="AC9" s="14"/>
       <c r="AD9" s="14">
         <f t="shared" si="7"/>
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="AE9" s="15"/>
       <c r="AF9" s="14"/>
       <c r="AG9" s="14">
         <f t="shared" si="8"/>
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="AH9" s="15"/>
       <c r="AI9" s="14"/>
       <c r="AJ9" s="14">
         <f t="shared" si="9"/>
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="AK9" s="15"/>
       <c r="AL9" s="14"/>
       <c r="AM9" s="14">
         <f t="shared" si="10"/>
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="AN9" s="15"/>
       <c r="AO9" s="14"/>
       <c r="AP9" s="14">
         <f t="shared" si="11"/>
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="AQ9" s="15"/>
       <c r="AR9" s="14"/>
       <c r="AS9" s="14">
         <f t="shared" si="12"/>
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="AT9" s="15"/>
       <c r="AU9" s="14"/>
       <c r="AV9" s="14">
         <f t="shared" si="13"/>
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="AW9" s="15"/>
       <c r="AX9" s="14"/>
       <c r="AY9" s="14">
         <f>AV9-AX9</f>
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="AZ9" s="14"/>
       <c r="BA9" s="14">
         <f t="shared" ref="BA9:BA27" si="14">AY9-AZ9</f>
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="BB9" s="14"/>
       <c r="BC9" s="14">
         <f t="shared" ref="BC9:BC27" si="15">BA9-BB9</f>
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="BD9" s="14"/>
       <c r="BE9" s="14">
         <f t="shared" ref="BE9:BE27" si="16">BC9-BD9</f>
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="BF9" s="14"/>
       <c r="BG9" s="14">
         <f t="shared" ref="BG9:BG27" si="17">BE9-BF9</f>
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="BH9" s="36">
         <f t="shared" ref="BH9:BH27" si="18">H9+K9+N9+Q9+T9+W9+Z9+AC9+AF9+AI9+AL9+AO9+AR9+AU9+AX9+AZ9+BB9+BD9+BF9</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BI9" s="36">
         <f>G9-BH9</f>
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="10" spans="2:62" s="25" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
@@ -1700,13 +1703,13 @@
       <c r="B11" s="26"/>
       <c r="C11" s="21"/>
       <c r="D11" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E11" s="47" t="s">
         <v>43</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="G11" s="27">
         <v>15</v>
@@ -1765,68 +1768,74 @@
         <v>15</v>
       </c>
       <c r="AH11" s="23"/>
-      <c r="AI11" s="23"/>
+      <c r="AI11" s="23">
+        <v>3</v>
+      </c>
       <c r="AJ11" s="23">
         <f t="shared" si="9"/>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="AK11" s="23"/>
       <c r="AL11" s="23"/>
       <c r="AM11" s="23">
         <f t="shared" si="10"/>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="AN11" s="23"/>
       <c r="AO11" s="23"/>
       <c r="AP11" s="23">
         <f t="shared" si="11"/>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="AQ11" s="23"/>
       <c r="AR11" s="23"/>
       <c r="AS11" s="23">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="AT11" s="23"/>
-      <c r="AU11" s="23"/>
+      <c r="AU11" s="23">
+        <v>1</v>
+      </c>
       <c r="AV11" s="23">
         <f t="shared" si="13"/>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="AW11" s="23"/>
       <c r="AX11" s="23"/>
       <c r="AY11" s="23">
         <f>AV11-AX11</f>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="AZ11" s="23"/>
       <c r="BA11" s="23">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="BB11" s="23"/>
       <c r="BC11" s="23">
         <f t="shared" si="15"/>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="BD11" s="23"/>
       <c r="BE11" s="23">
         <f t="shared" si="16"/>
-        <v>15</v>
-      </c>
-      <c r="BF11" s="23"/>
+        <v>11</v>
+      </c>
+      <c r="BF11" s="23">
+        <v>2</v>
+      </c>
       <c r="BG11" s="23">
         <f t="shared" si="17"/>
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="BH11" s="36">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="BI11" s="36">
         <f>G11-BH11</f>
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="BJ11" s="2"/>
     </row>
@@ -1834,13 +1843,13 @@
       <c r="B12" s="26"/>
       <c r="C12" s="21"/>
       <c r="D12" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E12" s="47" t="s">
         <v>43</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="G12" s="27">
         <v>3</v>
@@ -1949,27 +1958,29 @@
         <f t="shared" si="16"/>
         <v>3</v>
       </c>
-      <c r="BF12" s="23"/>
+      <c r="BF12" s="23">
+        <v>2.5</v>
+      </c>
       <c r="BG12" s="23">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="BH12" s="36">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="BI12" s="36">
         <f>G12-BH12</f>
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="BJ12" s="2"/>
     </row>
     <row r="13" spans="2:62" s="25" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B13" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
@@ -2038,13 +2049,13 @@
       <c r="B14" s="26"/>
       <c r="C14" s="21"/>
       <c r="D14" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E14" s="47" t="s">
         <v>43</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="G14" s="27">
         <v>15</v>
@@ -2133,38 +2144,46 @@
         <v>15</v>
       </c>
       <c r="AW14" s="23"/>
-      <c r="AX14" s="23"/>
+      <c r="AX14" s="23">
+        <v>4</v>
+      </c>
       <c r="AY14" s="23">
         <f t="shared" si="19"/>
-        <v>15</v>
-      </c>
-      <c r="AZ14" s="23"/>
+        <v>11</v>
+      </c>
+      <c r="AZ14" s="23">
+        <v>5</v>
+      </c>
       <c r="BA14" s="23">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="BB14" s="23"/>
       <c r="BC14" s="23">
         <f t="shared" si="15"/>
-        <v>15</v>
-      </c>
-      <c r="BD14" s="23"/>
+        <v>6</v>
+      </c>
+      <c r="BD14" s="23">
+        <v>4</v>
+      </c>
       <c r="BE14" s="23">
         <f t="shared" si="16"/>
-        <v>15</v>
-      </c>
-      <c r="BF14" s="23"/>
+        <v>2</v>
+      </c>
+      <c r="BF14" s="23">
+        <v>1</v>
+      </c>
       <c r="BG14" s="23">
         <f t="shared" si="17"/>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="BH14" s="36">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="BI14" s="36">
         <f>G14-BH14</f>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="BJ14" s="2"/>
     </row>
@@ -2172,13 +2191,13 @@
       <c r="B15" s="26"/>
       <c r="C15" s="21"/>
       <c r="D15" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E15" s="47" t="s">
         <v>43</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="G15" s="27">
         <v>3</v>
@@ -2287,18 +2306,20 @@
         <f t="shared" si="16"/>
         <v>3</v>
       </c>
-      <c r="BF15" s="23"/>
+      <c r="BF15" s="23">
+        <v>2.5</v>
+      </c>
       <c r="BG15" s="23">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="BH15" s="36">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="BI15" s="36">
         <f>G15-BH15</f>
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="BJ15" s="2"/>
     </row>
@@ -2344,16 +2365,16 @@
       <c r="AJ16" s="23"/>
       <c r="AK16" s="31"/>
       <c r="AL16" s="31"/>
-      <c r="AM16" s="23"/>
+      <c r="AM16" s="31"/>
       <c r="AN16" s="31"/>
       <c r="AO16" s="31"/>
-      <c r="AP16" s="23"/>
+      <c r="AP16" s="31"/>
       <c r="AQ16" s="31"/>
       <c r="AR16" s="31"/>
-      <c r="AS16" s="23"/>
+      <c r="AS16" s="31"/>
       <c r="AT16" s="31"/>
       <c r="AU16" s="31"/>
-      <c r="AV16" s="23"/>
+      <c r="AV16" s="31"/>
       <c r="AW16" s="31"/>
       <c r="AX16" s="31"/>
       <c r="AY16" s="23"/>
@@ -2373,13 +2394,13 @@
       <c r="B17" s="34"/>
       <c r="C17" s="29"/>
       <c r="D17" s="28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E17" s="31" t="s">
         <v>42</v>
       </c>
       <c r="F17" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G17" s="35">
         <v>15</v>
@@ -2519,13 +2540,13 @@
       <c r="B18" s="34"/>
       <c r="C18" s="29"/>
       <c r="D18" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E18" s="31" t="s">
         <v>42</v>
       </c>
       <c r="F18" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G18" s="35">
         <v>3</v>
@@ -2722,13 +2743,13 @@
       <c r="B20" s="34"/>
       <c r="C20" s="29"/>
       <c r="D20" s="28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E20" s="31" t="s">
         <v>42</v>
       </c>
       <c r="F20" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G20" s="35">
         <v>15</v>
@@ -2866,13 +2887,13 @@
       <c r="B21" s="34"/>
       <c r="C21" s="29"/>
       <c r="D21" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E21" s="31" t="s">
         <v>42</v>
       </c>
       <c r="F21" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G21" s="35">
         <v>3</v>
@@ -3000,10 +3021,10 @@
     </row>
     <row r="22" spans="2:62" s="42" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C22" s="38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D22" s="39"/>
       <c r="E22" s="39"/>
@@ -3069,13 +3090,13 @@
       <c r="B23" s="43"/>
       <c r="C23" s="38"/>
       <c r="D23" s="37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E23" s="37" t="s">
         <v>46</v>
       </c>
       <c r="F23" s="43" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G23" s="44">
         <v>15</v>
@@ -3213,13 +3234,13 @@
       <c r="B24" s="43"/>
       <c r="C24" s="38"/>
       <c r="D24" s="37" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E24" s="37" t="s">
         <v>46</v>
       </c>
       <c r="F24" s="43" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G24" s="44">
         <v>3</v>
@@ -3349,10 +3370,10 @@
     </row>
     <row r="25" spans="2:62" s="42" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="37" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C25" s="38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D25" s="39"/>
       <c r="E25" s="39"/>
@@ -3418,13 +3439,13 @@
       <c r="B26" s="43"/>
       <c r="C26" s="38"/>
       <c r="D26" s="37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E26" s="37" t="s">
         <v>46</v>
       </c>
       <c r="F26" s="40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G26" s="44">
         <v>15</v>
@@ -3556,13 +3577,13 @@
       <c r="B27" s="43"/>
       <c r="C27" s="38"/>
       <c r="D27" s="37" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E27" s="37" t="s">
         <v>46</v>
       </c>
       <c r="F27" s="40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G27" s="44">
         <v>3</v>
@@ -3754,6 +3775,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="BH4:BI4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="BB4:BC4"/>
+    <mergeCell ref="BD4:BE4"/>
+    <mergeCell ref="BF4:BG4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -3765,15 +3795,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="BH4:BI4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="BB4:BC4"/>
-    <mergeCell ref="BD4:BE4"/>
-    <mergeCell ref="BF4:BG4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="50" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -3798,7 +3819,7 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.42578125" style="4" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" style="4" customWidth="1"/>

</xml_diff>